<commit_message>
Added most recent xls files
</commit_message>
<xml_diff>
--- a/datafiles-2017/xlsfiles/Blood_lead2011to2015_cdc.xlsx
+++ b/datafiles-2017/xlsfiles/Blood_lead2011to2015_cdc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="14535"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Blood_Lead_Level" sheetId="1" r:id="rId1"/>
+    <sheet name="blood_lead" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Blood_Lead_Level">Blood_Lead_Level!$A$1:$AE$31</definedName>
+    <definedName name="blood_lead">blood_lead!$A$1:$AE$31</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -38,7 +38,7 @@
     <t>_ebll_c2015</t>
   </si>
   <si>
-    <t>_ebll_5yavg</t>
+    <t>_ebll_c1115</t>
   </si>
   <si>
     <t>_w_ebll_c2011</t>
@@ -56,7 +56,7 @@
     <t>_w_ebll_c2015</t>
   </si>
   <si>
-    <t>_w_ebll_5yavg</t>
+    <t>_w_ebll_c1115</t>
   </si>
   <si>
     <t>_b_ebll_c2011</t>
@@ -74,7 +74,7 @@
     <t>_b_ebll_c2015</t>
   </si>
   <si>
-    <t>_b_ebll_5yavg</t>
+    <t>_b_ebll_c1115</t>
   </si>
   <si>
     <t>_a_ebll_c2011</t>
@@ -92,7 +92,7 @@
     <t>_a_ebll_c2015</t>
   </si>
   <si>
-    <t>_a_ebll_5yavg</t>
+    <t>_a_ebll_c1115</t>
   </si>
   <si>
     <t>_o_ebll_c2011</t>
@@ -110,7 +110,7 @@
     <t>_o_ebll_c2015</t>
   </si>
   <si>
-    <t>_o_ebll_5yavg</t>
+    <t>_o_ebll_c1115</t>
   </si>
   <si>
     <t>Bellaire Puritas Community Dev. Corp.</t>
@@ -576,7 +576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3373,5 +3373,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>